<commit_message>
add joint bilateral fillter
</commit_message>
<xml_diff>
--- a/OpenCP/birateralFilter/graph_birateral.xlsx
+++ b/OpenCP/birateralFilter/graph_birateral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fukushima\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fukushima\Documents\GitHub\OpenCP\OpenCP\birateralFilter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -729,11 +729,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533916968"/>
-        <c:axId val="533916184"/>
+        <c:axId val="251518224"/>
+        <c:axId val="251005944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533916968"/>
+        <c:axId val="251518224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +848,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533916184"/>
+        <c:crossAx val="251005944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533916184"/>
+        <c:axId val="251005944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -974,7 +974,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533916968"/>
+        <c:crossAx val="251518224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1647,16 +1647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1941,15 +1941,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="G2" sqref="G2:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1982,8 +1982,12 @@
       <c r="E2">
         <v>5.6042799999999997E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G2">
+        <f>B2/C2</f>
+        <v>1.2358634408986409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1999,8 +2003,12 @@
       <c r="E3">
         <v>0.32616899999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G3">
+        <f t="shared" ref="G3:G31" si="0">B3/C3</f>
+        <v>1.0912305038017045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2016,8 +2024,12 @@
       <c r="E4">
         <v>1.0692200000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1.7235948244607822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2033,8 +2045,12 @@
       <c r="E5">
         <v>2.1970700000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.6329383183346433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2050,8 +2066,12 @@
       <c r="E6">
         <v>3.5293000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>3.2620026692637878</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2067,8 +2087,12 @@
       <c r="E7">
         <v>5.48332</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.5731344539330165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2084,8 +2108,12 @@
       <c r="E8">
         <v>7.5522799999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.0124249397808169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2101,8 +2129,12 @@
       <c r="E9">
         <v>9.9095499999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3.1926294609763848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2118,8 +2150,12 @@
       <c r="E10">
         <v>12.8607</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3.4730154383768839</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2135,8 +2171,12 @@
       <c r="E11">
         <v>16.240100000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3.7219489701813715</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2152,8 +2192,12 @@
       <c r="E12">
         <v>20.0398</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.9042254559869458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2169,8 +2213,12 @@
       <c r="E13">
         <v>23.8079</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3.961465157949188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2186,8 +2234,12 @@
       <c r="E14">
         <v>27.8443</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>3.7973072619193928</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2203,8 +2255,12 @@
       <c r="E15">
         <v>33.192900000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>4.0632332425526485</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2220,8 +2276,12 @@
       <c r="E16">
         <v>38.374299999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>4.0724251108092293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2237,8 +2297,12 @@
       <c r="E17">
         <v>43.904800000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>4.0307792670547089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2254,8 +2318,12 @@
       <c r="E18">
         <v>49.343899999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>3.9935396188853685</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2271,8 +2339,12 @@
       <c r="E19">
         <v>55.393000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>3.9660508617413286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2288,8 +2360,12 @@
       <c r="E20">
         <v>61.995199999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>3.9363917564193343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2305,8 +2381,12 @@
       <c r="E21">
         <v>69.046499999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>4.0642627974907821</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2322,8 +2402,12 @@
       <c r="E22">
         <v>76.785799999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>3.9786667464544312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2339,8 +2423,12 @@
       <c r="E23">
         <v>83.958699999999993</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>4.0126299529363392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2356,8 +2444,12 @@
       <c r="E24">
         <v>92.229399999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3.9352738715704589</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2373,8 +2465,12 @@
       <c r="E25">
         <v>100.642</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3.970924074562364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2390,8 +2486,12 @@
       <c r="E26">
         <v>109.217</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>3.6822714670577672</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2407,8 +2507,12 @@
       <c r="E27">
         <v>119.184</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>3.9033991946811502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2424,8 +2528,12 @@
       <c r="E28">
         <v>128.91900000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>4.0184663382825185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2441,8 +2549,12 @@
       <c r="E29">
         <v>138.072</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>3.8711207459118415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2458,8 +2570,12 @@
       <c r="E30">
         <v>148.01400000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>4.0785713857821495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2474,6 +2590,10 @@
       </c>
       <c r="E31">
         <v>158.34399999999999</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>3.8920567671749415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>